<commit_message>
Revert "Merge branch 'develop' into develop_opi"
This reverts commit c89a1e5bfea52ee82e33d08eee52c95a78db56e3.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/candidatures_template.xlsx
+++ b/src/main/resources/template/candidatures_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -280,6 +280,9 @@
     <t>Présél. Lieu&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
+    <t>${cand.lastTypeDecision.preselectDateTypeDecCand}</t>
+  </si>
+  <si>
     <t>${cand.lastTypeDecision.preselectLieuTypeDecCand}</t>
   </si>
   <si>
@@ -307,28 +310,13 @@
     <t>&lt;jt:hideCols test="${userAnnulHide}"&gt;Annulé par&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
+    <t>&lt;jt:if test="${cand.temAcceptCand!=null}"&gt;&lt;jt:if test="${cand.temAcceptCand}" then="CONFIRMATION" else="DESISTEMENT"/&gt;&lt;/jt:if&gt;</t>
+  </si>
+  <si>
     <t>${cand.userAnnulCand}&lt;/jt:forEach&gt;</t>
   </si>
   <si>
     <t>${cand.datAnnulCandStr}</t>
-  </si>
-  <si>
-    <t>${cand.datNewConfirmCandStr}</t>
-  </si>
-  <si>
-    <t>${cand.datNewRetourCandStr}</t>
-  </si>
-  <si>
-    <t>&lt;jt:if test="${cand.temAcceptCand!=null}"&gt;&lt;jt:if test="${cand.temAcceptCand}" then="CONFIRMATION" else="DESISTEMENT"/&gt;&lt;/jt:if&gt;</t>
-  </si>
-  <si>
-    <t>${cand.lastTypeDecision.preselectDateTypeDecCandStr}</t>
-  </si>
-  <si>
-    <t>&lt;jt:hideCols test="${datNewConfirmHide}"&gt;Date confirm. manuelle/LC&lt;/jt:hideCols&gt;</t>
-  </si>
-  <si>
-    <t>&lt;jt:hideCols test="${datNewRetourHide}"&gt;Date retour manuelle&lt;/jt:hideCols&gt;</t>
   </si>
 </sst>
 </file>
@@ -411,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -424,7 +412,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,12 +713,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -764,11 +751,11 @@
     <col min="39" max="39" width="15.42578125" style="4" customWidth="1"/>
     <col min="40" max="46" width="22" style="4" customWidth="1"/>
     <col min="47" max="47" width="18.42578125" style="4" customWidth="1"/>
-    <col min="48" max="50" width="28.28515625" style="4" customWidth="1"/>
-    <col min="51" max="51" width="16.5703125" customWidth="1"/>
+    <col min="48" max="48" width="28.28515625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -836,10 +823,10 @@
         <v>24</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>13</v>
@@ -911,22 +898,16 @@
         <v>55</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>103</v>
+        <v>35</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -994,10 +975,10 @@
         <v>43</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>7</v>
@@ -1057,36 +1038,30 @@
         <v>51</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="AS2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT2" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="AU2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="AV2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX2" t="s">
         <v>99</v>
       </c>
-      <c r="AW2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="AX2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>97</v>
-      </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1135,10 +1110,8 @@
       <c r="AT3" s="6"/>
       <c r="AU3" s="6"/>
       <c r="AV3" s="6"/>
-      <c r="AW3" s="6"/>
-      <c r="AX3" s="6"/>
-      <c r="AY3" s="7"/>
-      <c r="AZ3" s="7"/>
+      <c r="AW3" s="7"/>
+      <c r="AX3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>